<commit_message>
Add slick slider + preview on post deal
</commit_message>
<xml_diff>
--- a/rendu_projet/Rendu-Projet-Part1-BRUNEL-LEMETAYER.xlsx
+++ b/rendu_projet/Rendu-Projet-Part1-BRUNEL-LEMETAYER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brufl\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brufl\projets\projets_lp\php\dealabs\rendu_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583CE2A6-6D50-415D-B681-8796C03C6EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FE91A7-4D1A-42FA-9EFA-F479F6CE9C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A58EC350-CF33-BC4F-BC06-897311A7761F}"/>
   </bookViews>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F401AA-F8B3-C845-98CB-91317ACEBECA}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>